<commit_message>
05.11.2022 tarihli ders örneğidir.
</commit_message>
<xml_diff>
--- a/AribilgiWebProject/Docs/WebSiteDatabaseYapisi.xlsx
+++ b/AribilgiWebProject/Docs/WebSiteDatabaseYapisi.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -84,18 +84,6 @@
   </si>
   <si>
     <t>TagCode</t>
-  </si>
-  <si>
-    <t>Deri</t>
-  </si>
-  <si>
-    <t>Canta</t>
-  </si>
-  <si>
-    <t>Ayakkabı</t>
-  </si>
-  <si>
-    <t>Elektrik</t>
   </si>
 </sst>
 </file>
@@ -604,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +605,7 @@
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -627,17 +615,8 @@
       <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -647,17 +626,8 @@
       <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -667,17 +637,8 @@
       <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -687,34 +648,16 @@
       <c r="G4" t="s">
         <v>19</v>
       </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-      <c r="K5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -722,47 +665,47 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
         <v>14</v>
       </c>

</xml_diff>